<commit_message>
Add ppt composer to Figure 1 folder and make small tweaks
</commit_message>
<xml_diff>
--- a/LiteratureSynthesis/FigsFeb2022/Figure1-LakeUrmiaTrends/Figure1-LakeUrmiaTrends.xlsx
+++ b/LiteratureSynthesis/FigsFeb2022/Figure1-LakeUrmiaTrends/Figure1-LakeUrmiaTrends.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\Iran\UrmiaCoding\LiteratureSynthesis\FigsFeb2022\Figure1-LakeUrmiaTrends\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8033216-42CD-4FC9-A4EB-34C3E2221E23}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4521719-7449-45BC-A264-BE639DBAB116}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6230" xr2:uid="{06537FE8-0E15-0049-87D1-1226BA0277C8}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="34">
   <si>
     <t>Lake level (m)</t>
   </si>
@@ -324,9 +324,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -339,6 +336,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -348,10 +348,13 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF008000"/>
+      <color rgb="FFFFAC75"/>
+      <color rgb="FF3D87FF"/>
+      <color rgb="FF2857FF"/>
       <color rgb="FF85DFFF"/>
       <color rgb="FF003399"/>
       <color rgb="FF990000"/>
-      <color rgb="FF008000"/>
       <color rgb="FF009900"/>
     </mruColors>
   </colors>
@@ -693,7 +696,24 @@
                       <a:srgbClr val="003399"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>mm  Yr </a:t>
+                  <a:t>Precip.</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="1">
+                    <a:solidFill>
+                      <a:srgbClr val="003399"/>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="1">
+                    <a:solidFill>
+                      <a:srgbClr val="003399"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>(mm  Yr </a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" sz="1200" b="1" baseline="30000">
@@ -702,6 +722,14 @@
                     </a:solidFill>
                   </a:rPr>
                   <a:t>-1</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="003399"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US" sz="1200" b="1">
                   <a:solidFill>
@@ -715,8 +743,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="5.0895645440811085E-2"/>
-              <c:y val="0.53469311642470119"/>
+              <c:x val="4.7062897755780306E-2"/>
+              <c:y val="0.60927345312458137"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1134,7 +1162,7 @@
           <c:spPr>
             <a:ln w="22225" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="85DFFF"/>
+                <a:srgbClr val="008000"/>
               </a:solidFill>
               <a:prstDash val="sysDash"/>
               <a:round/>
@@ -1146,11 +1174,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="85DFFF"/>
+                <a:srgbClr val="008000"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:srgbClr val="85DFFF"/>
+                  <a:srgbClr val="008000"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1496,7 +1524,7 @@
                 <a:pPr>
                   <a:defRPr sz="1300" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:srgbClr val="85DFFF"/>
+                      <a:srgbClr val="008000"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1506,7 +1534,7 @@
                 <a:r>
                   <a:rPr lang="en-US" sz="1300" b="1">
                     <a:solidFill>
-                      <a:srgbClr val="85DFFF"/>
+                      <a:srgbClr val="008000"/>
                     </a:solidFill>
                   </a:rPr>
                   <a:t>Irrigated  Farms  (km</a:t>
@@ -1514,7 +1542,7 @@
                 <a:r>
                   <a:rPr lang="en-US" sz="1300" b="1" baseline="30000">
                     <a:solidFill>
-                      <a:srgbClr val="85DFFF"/>
+                      <a:srgbClr val="008000"/>
                     </a:solidFill>
                   </a:rPr>
                   <a:t>2</a:t>
@@ -1522,7 +1550,7 @@
                 <a:r>
                   <a:rPr lang="en-US" sz="1300" b="1">
                     <a:solidFill>
-                      <a:srgbClr val="85DFFF"/>
+                      <a:srgbClr val="008000"/>
                     </a:solidFill>
                   </a:rPr>
                   <a:t>)</a:t>
@@ -1534,8 +1562,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.96300586359948437"/>
-              <c:y val="0.17706992536753458"/>
+              <c:x val="0.96300586797641941"/>
+              <c:y val="8.3770720083866587E-2"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1553,7 +1581,7 @@
               <a:pPr>
                 <a:defRPr sz="1300" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:srgbClr val="85DFFF"/>
+                    <a:srgbClr val="008000"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -1585,7 +1613,7 @@
             <a:pPr>
               <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:srgbClr val="85DFFF"/>
+                  <a:srgbClr val="008000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1611,7 +1639,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="924065520"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="1500"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -3220,8 +3248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5CCAE1-FD26-4BA9-BA83-036CB80FA816}">
   <dimension ref="A1:AQ50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+    <sheetView tabSelected="1" topLeftCell="F5" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="U33" sqref="U33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3238,38 +3266,38 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="51.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
     </row>
     <row r="3" spans="1:43" s="1" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="28" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="29" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="3"/>

</xml_diff>